<commit_message>
resolved activity redirecting problem
</commit_message>
<xml_diff>
--- a/backend/static/database/activities.xlsx
+++ b/backend/static/database/activities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoome\OneDrive - Indian Institute of Science\Desktop\Gen AI\backend\static\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indianinstituteofscience-my.sharepoint.com/personal/saumysharan_iisc_ac_in/Documents/Desktop/projects/Gen AI/backend/static/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA67D17D-FB66-4EFF-A8A2-248F36B12460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FA67D17D-FB66-4EFF-A8A2-248F36B12460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8966FBD4-32E2-46FA-A638-700A17E354F3}"/>
   <bookViews>
-    <workbookView xWindow="11205" yWindow="3360" windowWidth="17715" windowHeight="11235" xr2:uid="{D0293FCB-4074-4066-9B35-6C85CF30C739}"/>
+    <workbookView xWindow="11085" yWindow="3360" windowWidth="17715" windowHeight="11235" xr2:uid="{D0293FCB-4074-4066-9B35-6C85CF30C739}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,14 +125,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,6 +147,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,7 +473,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,14 +515,8 @@
       <c r="C2" s="2">
         <v>100</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2">
         <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -532,8 +529,14 @@
       <c r="C3" s="2">
         <v>500</v>
       </c>
-      <c r="D3" s="4">
-        <v>5</v>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -546,7 +549,7 @@
       <c r="C4" s="2">
         <v>600</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>15</v>
       </c>
     </row>
@@ -560,7 +563,7 @@
       <c r="C5" s="2">
         <v>100</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>1</v>
       </c>
     </row>
@@ -574,7 +577,7 @@
       <c r="C6" s="2">
         <v>300</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>30</v>
       </c>
     </row>
@@ -588,7 +591,7 @@
       <c r="C7" s="2">
         <v>100</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>15</v>
       </c>
     </row>
@@ -602,7 +605,7 @@
       <c r="C8" s="2">
         <v>100</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>15</v>
       </c>
     </row>
@@ -616,7 +619,7 @@
       <c r="C9" s="2">
         <v>600</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improved ui and added flash message system
</commit_message>
<xml_diff>
--- a/backend/static/database/activities.xlsx
+++ b/backend/static/database/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indianinstituteofscience-my.sharepoint.com/personal/saumysharan_iisc_ac_in/Documents/Desktop/projects/Gen AI/backend/static/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FA67D17D-FB66-4EFF-A8A2-248F36B12460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8966FBD4-32E2-46FA-A638-700A17E354F3}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{FA67D17D-FB66-4EFF-A8A2-248F36B12460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89F9B427-6738-4EAF-80AC-8AC27F3F76CC}"/>
   <bookViews>
-    <workbookView xWindow="11085" yWindow="3360" windowWidth="17715" windowHeight="11235" xr2:uid="{D0293FCB-4074-4066-9B35-6C85CF30C739}"/>
+    <workbookView xWindow="3720" yWindow="6960" windowWidth="17715" windowHeight="11235" xr2:uid="{D0293FCB-4074-4066-9B35-6C85CF30C739}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -84,6 +84,48 @@
   </si>
   <si>
     <t>How do you feel after completing the meditation?</t>
+  </si>
+  <si>
+    <t>Journaling about things you're grateful for can improve your mental health and shift your focus to positive aspects of your life. Spend 5-10 minutes writing down at least three things you're grateful for today.</t>
+  </si>
+  <si>
+    <t>How do you feel after reflecting on the things you're grateful for?</t>
+  </si>
+  <si>
+    <t>Physical exercise can boost your mood and reduce stress. Engage in any form of exercise you enjoy, such as walking, jogging, yoga, or dancing, for at least 15-30 minutes.</t>
+  </si>
+  <si>
+    <t>How do you feel physically and mentally after completing your exercise routine?</t>
+  </si>
+  <si>
+    <t>Positive affirmations can help you build self-esteem and improve your mindset. Take a moment to write or say a few positive affirmations about yourself or your abilities.</t>
+  </si>
+  <si>
+    <t>How did the affirmations make you feel? Did they impact your self-perception?</t>
+  </si>
+  <si>
+    <t>Disconnecting from your phone, social media, or other digital distractions can improve focus and reduce stress. Take at least 30 minutes today to unplug and spend time doing something offline.</t>
+  </si>
+  <si>
+    <t>How did you feel after spending time away from digital devices? Did you notice any change in your focus or mood?</t>
+  </si>
+  <si>
+    <t>Practice mindful eating by focusing on the flavors, textures, and smells of your food. Avoid distractions and take your time to enjoy each bite during your meal.</t>
+  </si>
+  <si>
+    <t>How did practicing mindful eating affect your enjoyment of the meal? Did you notice any changes in your eating habits or how you felt afterward?</t>
+  </si>
+  <si>
+    <t>Engage in a creative activity such as drawing, painting, writing, or playing an instrument. Allow yourself to express your emotions and thoughts through your chosen medium for at least 15-30 minutes.</t>
+  </si>
+  <si>
+    <t>How did engaging in creative expression make you feel? Did you discover any new thoughts or emotions during the process?</t>
+  </si>
+  <si>
+    <t>It's important to be aware of how you're feeling throughout the day. Take a few minutes to pause and assess your current mood. Reflect on any emotions you're experiencing and consider their causes.</t>
+  </si>
+  <si>
+    <t>How do you feel right now? What emotions are you experiencing, and why?</t>
   </si>
 </sst>
 </file>
@@ -473,7 +515,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +558,13 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -552,6 +600,12 @@
       <c r="D4">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -564,7 +618,13 @@
         <v>100</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -580,6 +640,12 @@
       <c r="D6">
         <v>30</v>
       </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -594,6 +660,12 @@
       <c r="D7">
         <v>15</v>
       </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -608,6 +680,12 @@
       <c r="D8">
         <v>15</v>
       </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -621,6 +699,12 @@
       </c>
       <c r="D9">
         <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added leaderboard and progress bar
</commit_message>
<xml_diff>
--- a/backend/static/database/activities.xlsx
+++ b/backend/static/database/activities.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{FA67D17D-FB66-4EFF-A8A2-248F36B12460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89F9B427-6738-4EAF-80AC-8AC27F3F76CC}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="6960" windowWidth="17715" windowHeight="11235" xr2:uid="{D0293FCB-4074-4066-9B35-6C85CF30C739}"/>
+    <workbookView xWindow="6420" yWindow="4245" windowWidth="17715" windowHeight="11235" xr2:uid="{D0293FCB-4074-4066-9B35-6C85CF30C739}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -515,7 +515,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>